<commit_message>
populates DB and returns JSON
</commit_message>
<xml_diff>
--- a/Article.xlsx
+++ b/Article.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
-  <workbookPr defaultThemeVersion="202300"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aamirsangey/Documents/temp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\Project\Mind-Check\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B31CEF30-C123-FC4D-B642-FCEE8253BBB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3880" yWindow="3120" windowWidth="27240" windowHeight="16440" xr2:uid="{7F2B6B00-3CB9-DA45-827F-5F1D3CFA5077}"/>
+    <workbookView xWindow="3876" yWindow="3120" windowWidth="27240" windowHeight="16440"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -47,9 +46,6 @@
     <t>Depression</t>
   </si>
   <si>
-    <t xml:space="preserve">Scuidal </t>
-  </si>
-  <si>
     <t>Stress</t>
   </si>
   <si>
@@ -132,13 +128,16 @@
   </si>
   <si>
     <t>url</t>
+  </si>
+  <si>
+    <t>Suicidal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -513,54 +512,54 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2A68508-AB2C-844B-8BDB-2E8B02C6633F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="104.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="214.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="104.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="214.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
         <v>29</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>30</v>
       </c>
-      <c r="C1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -568,138 +567,138 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>20</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>21</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>0</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>2</v>
       </c>
       <c r="B11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
         <v>3</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C13" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
         <v>4</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>26</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
         <v>5</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C15" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C11" r:id="rId1" xr:uid="{83AD7C88-86B0-3748-81E6-AE4B6866F567}"/>
-    <hyperlink ref="C12" r:id="rId2" xr:uid="{E7BEE29D-B2A7-CE49-A564-1966A3C3F4E3}"/>
-    <hyperlink ref="C7" r:id="rId3" xr:uid="{4DBB6584-40FD-7D4D-ABC5-BCE2AFA8A32E}"/>
-    <hyperlink ref="C8" r:id="rId4" xr:uid="{18BB2DFF-3CCA-FF48-B898-B1DA42744CA7}"/>
-    <hyperlink ref="C14" r:id="rId5" xr:uid="{0E5290B2-84FA-9D48-9F75-807584459D5F}"/>
-    <hyperlink ref="C9" r:id="rId6" xr:uid="{DCFB91F8-8EAA-394F-80B9-5686EB71D0C5}"/>
+    <hyperlink ref="C11" r:id="rId1"/>
+    <hyperlink ref="C12" r:id="rId2"/>
+    <hyperlink ref="C7" r:id="rId3"/>
+    <hyperlink ref="C8" r:id="rId4"/>
+    <hyperlink ref="C14" r:id="rId5"/>
+    <hyperlink ref="C9" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>